<commit_message>
Updated the dummy data
</commit_message>
<xml_diff>
--- a/TransactionDeets.xlsx
+++ b/TransactionDeets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjjj8\OneDrive\Documents\GitHub\PortfolioProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149642D7-838D-4FA3-BE5B-95C9D1BF71BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B10922-3CFC-4ABC-BF34-AC76F13B6CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5556" yWindow="756" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>WAAREEENER.NS</t>
+  </si>
+  <si>
+    <t>HUDCO</t>
+  </si>
+  <si>
+    <t>HUDCO.NS</t>
   </si>
 </sst>
 </file>
@@ -75,7 +81,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -142,7 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -456,7 +462,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,8 +635,31 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45601</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5">
+        <v>50</v>
+      </c>
+      <c r="G7" s="9">
+        <v>214.5</v>
+      </c>
+      <c r="H7" s="9">
+        <f>PRODUCT(F7,G7)</f>
+        <v>10725</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G8" s="9"/>

</xml_diff>